<commit_message>
update (Cau Hoi + Cau Tra Loi) : Import
</commit_message>
<xml_diff>
--- a/File/CauHoi.xlsx
+++ b/File/CauHoi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\app-test-management\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3BB664-E5BA-4F23-86CF-46C06E34AFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB8AC1C-2645-4305-8B30-2D67B4EDECF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="1656" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
   </bookViews>
   <sheets>
     <sheet name="CauHoi" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Trắc nghiệm</t>
   </si>
@@ -59,29 +59,59 @@
     <t>is_DapAn</t>
   </si>
   <si>
-    <t>Kỹ thuật nào dưới đây được sử dụng để đảm bảo phần mềm đáp ứng đúng yêu cầu của khách hàng trước khi triển khai?</t>
-  </si>
-  <si>
-    <t>Kiểm thử phần mềm (Software Testing)</t>
-  </si>
-  <si>
     <t>MaCauHoi</t>
   </si>
   <si>
-    <t>Triển khai phần mềm (Software Deployment)</t>
-  </si>
-  <si>
     <t>Phân tích yêu cầu (Requirement Analysis)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bảo trì phần mềm (Software Maintenance)</t>
+    <t>Trong quy trình phát triển phần mềm, giai đoạn nào tập trung vào việc xác định các chức năng và ràng buộc của hệ thống?</t>
+  </si>
+  <si>
+    <t>Thiết kế hệ thống (System Design)</t>
+  </si>
+  <si>
+    <t>Lập trình (Programming)</t>
+  </si>
+  <si>
+    <t>Kiểm thử (Testing)</t>
+  </si>
+  <si>
+    <t>Trong mô hình thác nước (Waterfall), bước nào phải được hoàn thành trước khi chuyển sang bước tiếp theo?</t>
+  </si>
+  <si>
+    <t>Công cụ nào thường được sử dụng để quản lý phiên bản mã nguồn trong các dự án phần mềm?</t>
+  </si>
+  <si>
+    <t>Lập kế hoạch (Planning)</t>
+  </si>
+  <si>
+    <t>Yêu cầu (Requirement)</t>
+  </si>
+  <si>
+    <t>Triển khai (Deployment)</t>
+  </si>
+  <si>
+    <t>Tất cả các bước trên</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Jira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,13 +130,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,7 +169,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +506,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,16 +533,44 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -535,10 +585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058ACC3-48A7-4AF6-AFA5-49C9326BD118}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +600,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -564,10 +614,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,10 +625,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -597,9 +647,97 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update(CauHoi): import CauHoi (TN+Dien)
</commit_message>
<xml_diff>
--- a/File/CauHoi.xlsx
+++ b/File/CauHoi.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\app-test-management\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB8AC1C-2645-4305-8B30-2D67B4EDECF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA6A1B-ACC0-4176-994D-D2D0FBC85683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
+    <workbookView xWindow="30612" yWindow="1656" windowWidth="23256" windowHeight="12456" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
   </bookViews>
   <sheets>
     <sheet name="CauHoi" sheetId="1" r:id="rId1"/>
     <sheet name="CauTraLoi" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="DienTu" sheetId="5" r:id="rId3"/>
+    <sheet name="NoiTu" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Trắc nghiệm</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>Jira</t>
+  </si>
+  <si>
+    <t>ViTri</t>
+  </si>
+  <si>
+    <t>DapAnText</t>
+  </si>
+  <si>
+    <t>Mô hình (1) là một quy trình phát triển phần mềm, trong đó các giai đoạn như yêu cầu, thiết kế, triển khai và kiểm thử được thực hiện theo thứ tự tuần tự. (Thác nước)</t>
+  </si>
+  <si>
+    <t>Thác nước</t>
+  </si>
+  <si>
+    <t>Điền từ</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,79 +524,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565109B9-5A0C-4BC3-8014-9F412906A63E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="138.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="138.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
       <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
       <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058ACC3-48A7-4AF6-AFA5-49C9326BD118}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,14 +799,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666469A8-45EB-4A4F-B60E-01562F546214}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
done: Project but also error valid and logic
</commit_message>
<xml_diff>
--- a/File/CauHoi.xlsx
+++ b/File/CauHoi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\app-test-management\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA6A1B-ACC0-4176-994D-D2D0FBC85683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CB2257-99B6-4959-96C4-79B5A340D50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="1656" windowWidth="23256" windowHeight="12456" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{01CAA580-8AE9-42D4-B032-4AE9B1C99E91}"/>
   </bookViews>
   <sheets>
     <sheet name="CauHoi" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Trắc nghiệm</t>
   </si>
@@ -62,48 +62,12 @@
     <t>MaCauHoi</t>
   </si>
   <si>
-    <t>Phân tích yêu cầu (Requirement Analysis)</t>
-  </si>
-  <si>
-    <t>Trong quy trình phát triển phần mềm, giai đoạn nào tập trung vào việc xác định các chức năng và ràng buộc của hệ thống?</t>
-  </si>
-  <si>
-    <t>Thiết kế hệ thống (System Design)</t>
-  </si>
-  <si>
-    <t>Lập trình (Programming)</t>
-  </si>
-  <si>
-    <t>Kiểm thử (Testing)</t>
-  </si>
-  <si>
-    <t>Trong mô hình thác nước (Waterfall), bước nào phải được hoàn thành trước khi chuyển sang bước tiếp theo?</t>
-  </si>
-  <si>
-    <t>Công cụ nào thường được sử dụng để quản lý phiên bản mã nguồn trong các dự án phần mềm?</t>
-  </si>
-  <si>
-    <t>Lập kế hoạch (Planning)</t>
-  </si>
-  <si>
-    <t>Yêu cầu (Requirement)</t>
-  </si>
-  <si>
-    <t>Triển khai (Deployment)</t>
-  </si>
-  <si>
-    <t>Tất cả các bước trên</t>
-  </si>
-  <si>
     <t>Docker</t>
   </si>
   <si>
     <t>Git</t>
   </si>
   <si>
-    <t>Jenkins</t>
-  </si>
-  <si>
     <t>Jira</t>
   </si>
   <si>
@@ -113,16 +77,131 @@
     <t>DapAnText</t>
   </si>
   <si>
-    <t>Mô hình (1) là một quy trình phát triển phần mềm, trong đó các giai đoạn như yêu cầu, thiết kế, triển khai và kiểm thử được thực hiện theo thứ tự tuần tự. (Thác nước)</t>
-  </si>
-  <si>
-    <t>Thác nước</t>
-  </si>
-  <si>
-    <t>Điền từ</t>
-  </si>
-  <si>
-    <t>abc</t>
+    <t>Mô hình phát triển phần mềm nào phù hợp với dự án có yêu cầu thay đổi liên tục?</t>
+  </si>
+  <si>
+    <t>Yếu tố nào KHÔNG thuộc đặc điểm của phần mềm?</t>
+  </si>
+  <si>
+    <t>Trong vòng đời phát triển phần mềm, bước nào thường được thực hiện đầu tiên?</t>
+  </si>
+  <si>
+    <t>Công cụ nào sau đây thường được sử dụng để quản lý mã nguồn trong phát triển phần mềm?</t>
+  </si>
+  <si>
+    <t>Tài liệu nào thường được viết trong giai đoạn Phân tích yêu cầu?</t>
+  </si>
+  <si>
+    <t>Mô hình Agile nhấn mạnh yếu tố nào?</t>
+  </si>
+  <si>
+    <t>Nguyên tắc nào là cốt lõi trong phát triển phần mềm hướng đối tượng?</t>
+  </si>
+  <si>
+    <t>Kỹ thuật kiểm thử phần mềm nào dựa trên việc xem xét mã nguồn?</t>
+  </si>
+  <si>
+    <t>Thuật ngữ nào mô tả khả năng một hệ thống phần mềm có thể phát triển và mở rộng trong tương lai?</t>
+  </si>
+  <si>
+    <t>Mô hình Thác nước (Waterfall)</t>
+  </si>
+  <si>
+    <t>Mô hình Scrum</t>
+  </si>
+  <si>
+    <t>Mô hình V (V-Model)</t>
+  </si>
+  <si>
+    <t>Mô hình Big Bang</t>
+  </si>
+  <si>
+    <t>Phần mềm không hao mòn vật lý</t>
+  </si>
+  <si>
+    <t>Phần mềm có thể sao chép dễ dàng</t>
+  </si>
+  <si>
+    <t>Phần mềm cần bảo trì để sửa lỗi và nâng cấp tính năng</t>
+  </si>
+  <si>
+    <t>Phần mềm có thể bị rò rỉ qua oxi hóa</t>
+  </si>
+  <si>
+    <t>Kiểm thử phần mềm</t>
+  </si>
+  <si>
+    <t>Phân tích yêu cầu</t>
+  </si>
+  <si>
+    <t>Triển khai phần mềm</t>
+  </si>
+  <si>
+    <t>Bảo trì phần mềm</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
+    <t>Tài liệu đặc tả yêu cầu phần mềm (SRS)</t>
+  </si>
+  <si>
+    <t>Tài liệu kiểm thử phần mềm (Test Plan)</t>
+  </si>
+  <si>
+    <t>Tài liệu hướng dẫn sử dụng (User Manual)</t>
+  </si>
+  <si>
+    <t>Tài liệu cấu trúc mã nguồn (Code Structure)</t>
+  </si>
+  <si>
+    <t>Quy trình nghiêm ngặt</t>
+  </si>
+  <si>
+    <t>Tài liệu chi tiết</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàn thiện sản phẩm trước khi giao tiếp với khách hàng
+</t>
+  </si>
+  <si>
+    <t>Tương tác con người và thích ứng với thay đổi</t>
+  </si>
+  <si>
+    <t>Đóng gói, Kế thừa, Đa hình</t>
+  </si>
+  <si>
+    <t>Phân lớp, Lập trình song song, Tự động hóa</t>
+  </si>
+  <si>
+    <t>Tái sử dụng mã nguồn, Thiết kế module, Giảm độ phức tạp</t>
+  </si>
+  <si>
+    <t>Cả B và C</t>
+  </si>
+  <si>
+    <t>Kiểm thử hộp đen</t>
+  </si>
+  <si>
+    <t>Kiểm thử hộp trắng</t>
+  </si>
+  <si>
+    <t>Kiểm thử tích hợp</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống</t>
+  </si>
+  <si>
+    <t>Khả năng bảo trì (Maintainability)</t>
+  </si>
+  <si>
+    <t>Khả năng mở rộng (Scalability)</t>
+  </si>
+  <si>
+    <t>Khả năng tái sử dụng (Reusability)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Độ tin cậy (Reliability)</t>
   </si>
 </sst>
 </file>
@@ -173,13 +252,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +266,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565109B9-5A0C-4BC3-8014-9F412906A63E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,20 +623,20 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -561,8 +644,8 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -578,8 +661,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -595,8 +678,8 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -612,8 +695,8 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -622,11 +705,93 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -636,36 +801,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058ACC3-48A7-4AF6-AFA5-49C9326BD118}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -673,10 +838,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -684,10 +849,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -695,10 +860,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -706,10 +871,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -717,10 +882,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -728,10 +893,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -739,10 +904,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -750,10 +915,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -761,10 +926,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -772,10 +937,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -783,12 +948,276 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37">
         <v>0</v>
       </c>
     </row>
@@ -799,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666469A8-45EB-4A4F-B60E-01562F546214}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,38 +1242,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>